<commit_message>
esercizi da far valutare
all'interno della cartellla di lavoro ci sono entrambi gli esercizi, sia il 9 che l'11.
</commit_message>
<xml_diff>
--- a/esercizio 9 svolto.xlsx
+++ b/esercizio 9 svolto.xlsx
@@ -3,12 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{873C4E38-CB2B-4399-BF39-9FFE49B00A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8815AC7C-2561-4FAA-A87D-2EA606A1FD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E123DFDF-41E7-4503-B4AC-A725FA0C5974}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E123DFDF-41E7-4503-B4AC-A725FA0C5974}"/>
   </bookViews>
   <sheets>
     <sheet name="anagrafica_aziendale" sheetId="1" r:id="rId1"/>
+    <sheet name="orario_lavoro" sheetId="3" r:id="rId2"/>
+    <sheet name="Foglio1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
   <si>
     <t>Amministrazione</t>
   </si>
@@ -151,17 +153,63 @@
   </si>
   <si>
     <t>Funzione int</t>
+  </si>
+  <si>
+    <t>totale</t>
+  </si>
+  <si>
+    <t>Retr. Straordinario</t>
+  </si>
+  <si>
+    <t>Retrib. Oraria</t>
+  </si>
+  <si>
+    <t>totale ore</t>
+  </si>
+  <si>
+    <t>Domenica</t>
+  </si>
+  <si>
+    <t>Sabato</t>
+  </si>
+  <si>
+    <t>Venerdì</t>
+  </si>
+  <si>
+    <t>Giovedì</t>
+  </si>
+  <si>
+    <t>Mercoledì</t>
+  </si>
+  <si>
+    <t>Martedì</t>
+  </si>
+  <si>
+    <t>Lunedì</t>
+  </si>
+  <si>
+    <t>uscita</t>
+  </si>
+  <si>
+    <t>entrata</t>
+  </si>
+  <si>
+    <t>esercizio 11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="2">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="168" formatCode="#,##0.00\ _€"/>
+    <numFmt numFmtId="169" formatCode="[h]:mm:ss;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,8 +242,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,6 +266,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -252,11 +313,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -276,10 +338,26 @@
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Euro" xfId="1" xr:uid="{05E7F11F-6F36-4D5E-B619-68835A6DDD65}"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Valuta 2" xfId="2" xr:uid="{9526829A-9EBF-45CD-8B2B-CB0ECA532CBD}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
@@ -372,6 +450,116 @@
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="CasellaDiTesto 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBD3D317-80DF-4B27-9864-45C6B482EFD9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6096000" y="182880"/>
+          <a:ext cx="3048000" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPts val="2100"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1400"/>
+            <a:t>Calcolo orario lavoro</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPts val="2100"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1400"/>
+            <a:t>Retr.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1400" baseline="0"/>
+            <a:t> oraria 17,50</a:t>
+          </a:r>
+          <a:endParaRPr lang="it-IT" sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPts val="2100"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1400"/>
+            <a:t>Straordinario (oltre le</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="it-IT" sz="1400" baseline="0"/>
+            <a:t> 36 ore) 19,00</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPts val="1100"/>
+            </a:lnSpc>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -682,7 +870,7 @@
   </sheetPr>
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
@@ -1670,4 +1858,255 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAED7B-574F-4C1C-B9B7-E2299F7F0319}">
+  <dimension ref="B1:L23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="16.88671875" customWidth="1"/>
+    <col min="7" max="7" width="3" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C2" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B3" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="25">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D3" s="25">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E3" s="25">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F3" s="25">
+        <v>0.75</v>
+      </c>
+      <c r="H3" s="25">
+        <f t="shared" ref="H3:H9" si="0">SUM(F3-E3+D3-C3)</f>
+        <v>0.31944444444444436</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="25">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D4" s="25">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="H4" s="25">
+        <f t="shared" si="0"/>
+        <v>0.25000000000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="25">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="D5" s="25">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E5" s="25">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F5" s="25">
+        <v>0.75694444444444453</v>
+      </c>
+      <c r="H5" s="25">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="25">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="D6" s="25">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="E6" s="25">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F6" s="25">
+        <v>0.74305555555555547</v>
+      </c>
+      <c r="H6" s="25">
+        <f t="shared" si="0"/>
+        <v>0.34027777777777757</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="25">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="D7" s="25">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="E7" s="25">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F7" s="25">
+        <v>0.75347222222222221</v>
+      </c>
+      <c r="H7" s="25">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="25">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D8" s="25">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="H8" s="25">
+        <f t="shared" si="0"/>
+        <v>0.14583333333333331</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B9" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="H9" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F11" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="24">
+        <f>SUM(H9,H8,H7,H6,H5,H4,H3)</f>
+        <v>1.7222222222222221</v>
+      </c>
+      <c r="J11" s="23"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="H12" s="23">
+        <f>H11*24</f>
+        <v>41.333333333333329</v>
+      </c>
+      <c r="K12" s="22"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F13" s="21"/>
+      <c r="H13" s="21"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E14" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="19">
+        <v>17.5</v>
+      </c>
+      <c r="H14" s="1">
+        <f>H18-H15</f>
+        <v>630</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="E15" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="19">
+        <v>19</v>
+      </c>
+      <c r="H15" s="1">
+        <f>IF(H12&gt;36,(H12-36)*19, 0)</f>
+        <v>101.33333333333324</v>
+      </c>
+    </row>
+    <row r="18" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="F18" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" s="1">
+        <f>IF(H12&gt;36,F14*36+(H12-36)*F15,H12*F14)</f>
+        <v>731.33333333333326</v>
+      </c>
+      <c r="L18" s="17"/>
+    </row>
+    <row r="23" spans="5:12" x14ac:dyDescent="0.3">
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="H23" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B893E45-CD06-43B0-92EA-D0D91FCCCE62}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>